<commit_message>
Added 10 data points
</commit_message>
<xml_diff>
--- a/avida_mutations.xlsx
+++ b/avida_mutations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712341e5c6875785/Current Semester/BIO475/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{58458115-FBB3-7840-BCA8-D36F4C9B53B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8B158EB-A807-9E4D-B924-CDF695A83615}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{58458115-FBB3-7840-BCA8-D36F4C9B53B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49D23D22-2840-0F43-BD30-8C8D9B8CE8B9}"/>
   <bookViews>
-    <workbookView xWindow="16280" yWindow="460" windowWidth="20940" windowHeight="20180" xr2:uid="{734AC4CE-451D-F041-BA6E-6AFF42FD516B}"/>
+    <workbookView xWindow="39280" yWindow="1100" windowWidth="20940" windowHeight="20180" xr2:uid="{734AC4CE-451D-F041-BA6E-6AFF42FD516B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="291">
   <si>
     <t>organism_name</t>
   </si>
@@ -650,6 +650,36 @@
     <t>nomut_43</t>
   </si>
   <si>
+    <t>notose_71</t>
+  </si>
+  <si>
+    <t>notose_72</t>
+  </si>
+  <si>
+    <t>notose_73</t>
+  </si>
+  <si>
+    <t>notose_74</t>
+  </si>
+  <si>
+    <t>notose_75</t>
+  </si>
+  <si>
+    <t>notose_76</t>
+  </si>
+  <si>
+    <t>notose_77</t>
+  </si>
+  <si>
+    <t>notose_78</t>
+  </si>
+  <si>
+    <t>notose_79</t>
+  </si>
+  <si>
+    <t>notose_80</t>
+  </si>
+  <si>
     <t>whjagchmivznzbxbvmbzpfvfpwubypsmyuuobyufycvovrxguw</t>
   </si>
   <si>
@@ -795,6 +825,87 @@
   </si>
   <si>
     <t>nomut_70</t>
+  </si>
+  <si>
+    <t>wzcagccwyfvnyucucvdafcbnseccycqcifckqrncizvecaxgab</t>
+  </si>
+  <si>
+    <t>nomut_71</t>
+  </si>
+  <si>
+    <t>wzcagciqcuwcuvcicoazycqmccvbtyevrcxsrstiszvfaxxgab</t>
+  </si>
+  <si>
+    <t>wzcagclecuocqkcpconcyclrujvbtpcvrypsrmtmnzvfcaxgab</t>
+  </si>
+  <si>
+    <t>nomut_72</t>
+  </si>
+  <si>
+    <t>wzcagclecuocnkcpconcyclruzvjtpcvrypsrmtmnzvfcaxgab</t>
+  </si>
+  <si>
+    <t>notmut_73</t>
+  </si>
+  <si>
+    <t>wzcagciqiuwcuvticoazycqmccvbtyevrcxsrstiszvfaxxgab</t>
+  </si>
+  <si>
+    <t>wzcagcneduwrbkoovoncyfuovovojpcyulpizytbazvfcaxgab</t>
+  </si>
+  <si>
+    <t>wzcagcqeduwzbkdpcorcyfuoczwojrcvulplpmthczvfcaxgab</t>
+  </si>
+  <si>
+    <t>nomut_74</t>
+  </si>
+  <si>
+    <t>nomut_75</t>
+  </si>
+  <si>
+    <t>wzcagcqeduwzbkdpcorcyfuoczwojrcvulplpmthczvfclxgab</t>
+  </si>
+  <si>
+    <t>nomut_76</t>
+  </si>
+  <si>
+    <t>wzcagcqeduwcrkqpeorcefwoczvojrcvulplpmtpazvfcaxgab</t>
+  </si>
+  <si>
+    <t>wzcagcneduwrbkoovoncyfuovpvojpcyulpizyhbazvfcaxgab</t>
+  </si>
+  <si>
+    <t>nomut_77</t>
+  </si>
+  <si>
+    <t>wzcagcqeduwcrkqpcorcefwocrsojrcvulplpmtpazvfeaxgab</t>
+  </si>
+  <si>
+    <t>nomut_78</t>
+  </si>
+  <si>
+    <t>wzcagcnydfwrjxmokoncafuovpqcjqtyulpjzhhwazvfcaxgab</t>
+  </si>
+  <si>
+    <t>wzcaxcwgcuciufjnypvzywslkcvblicvlfweiseptzvfcajgab</t>
+  </si>
+  <si>
+    <t>nomut_79</t>
+  </si>
+  <si>
+    <t>wzcagcnednwibkohvoncnfuovpycjpcyulpuzthfazvfcaxgab</t>
+  </si>
+  <si>
+    <t>wzcagcwydfwrjxookoncafuovpqcjqtyulpjzhhwazvfcaxgab</t>
+  </si>
+  <si>
+    <t>wzcagcwydfwryxoskoncafooqpqcxqtyulpjzhhwazvfcaxgab</t>
+  </si>
+  <si>
+    <t>nomut_80</t>
+  </si>
+  <si>
+    <t>wzcagcwydfwrvxookoncafuovpqcjqtyulnjzhxwazvfcaxgab</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D558455-8CAF-9649-825D-30601F2953E4}">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141:D141"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2761,7 +2872,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B115" t="s">
         <v>136</v>
@@ -2770,12 +2881,12 @@
         <v>102</v>
       </c>
       <c r="D115" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B116" t="s">
         <v>136</v>
@@ -2784,12 +2895,12 @@
         <v>102</v>
       </c>
       <c r="D116" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B117" t="s">
         <v>136</v>
@@ -2798,12 +2909,12 @@
         <v>102</v>
       </c>
       <c r="D117" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B118" t="s">
         <v>136</v>
@@ -2812,12 +2923,12 @@
         <v>102</v>
       </c>
       <c r="D118" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="B119" t="s">
         <v>136</v>
@@ -2826,12 +2937,12 @@
         <v>102</v>
       </c>
       <c r="D119" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="B120" t="s">
         <v>136</v>
@@ -2840,12 +2951,12 @@
         <v>102</v>
       </c>
       <c r="D120" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
         <v>136</v>
@@ -2854,12 +2965,12 @@
         <v>102</v>
       </c>
       <c r="D121" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="B122" t="s">
         <v>136</v>
@@ -2868,12 +2979,12 @@
         <v>102</v>
       </c>
       <c r="D122" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="B123" t="s">
         <v>136</v>
@@ -2882,12 +2993,12 @@
         <v>102</v>
       </c>
       <c r="D123" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B124" t="s">
         <v>136</v>
@@ -2896,12 +3007,12 @@
         <v>102</v>
       </c>
       <c r="D124" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
         <v>136</v>
@@ -2910,12 +3021,12 @@
         <v>102</v>
       </c>
       <c r="D125" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="B126" t="s">
         <v>136</v>
@@ -2924,12 +3035,12 @@
         <v>102</v>
       </c>
       <c r="D126" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B127" t="s">
         <v>136</v>
@@ -2938,12 +3049,12 @@
         <v>102</v>
       </c>
       <c r="D127" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -2952,12 +3063,12 @@
         <v>102</v>
       </c>
       <c r="D128" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="B129" t="s">
         <v>136</v>
@@ -2966,12 +3077,12 @@
         <v>102</v>
       </c>
       <c r="D129" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -2980,12 +3091,12 @@
         <v>102</v>
       </c>
       <c r="D130" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B131" t="s">
         <v>136</v>
@@ -2994,12 +3105,12 @@
         <v>102</v>
       </c>
       <c r="D131" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
@@ -3008,12 +3119,12 @@
         <v>102</v>
       </c>
       <c r="D132" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B133" t="s">
         <v>136</v>
@@ -3022,12 +3133,12 @@
         <v>102</v>
       </c>
       <c r="D133" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B134" t="s">
         <v>136</v>
@@ -3036,12 +3147,12 @@
         <v>102</v>
       </c>
       <c r="D134" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
@@ -3050,12 +3161,12 @@
         <v>102</v>
       </c>
       <c r="D135" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
@@ -3064,12 +3175,12 @@
         <v>102</v>
       </c>
       <c r="D136" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B137" t="s">
         <v>136</v>
@@ -3078,12 +3189,12 @@
         <v>102</v>
       </c>
       <c r="D137" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B138" t="s">
         <v>136</v>
@@ -3092,12 +3203,12 @@
         <v>102</v>
       </c>
       <c r="D138" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="B139" t="s">
         <v>136</v>
@@ -3106,12 +3217,12 @@
         <v>102</v>
       </c>
       <c r="D139" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="B140" t="s">
         <v>136</v>
@@ -3120,12 +3231,12 @@
         <v>102</v>
       </c>
       <c r="D140" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="B141" t="s">
         <v>136</v>
@@ -3134,7 +3245,287 @@
         <v>102</v>
       </c>
       <c r="D141" t="s">
-        <v>218</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>205</v>
+      </c>
+      <c r="B142" t="s">
+        <v>137</v>
+      </c>
+      <c r="C142" t="s">
+        <v>38</v>
+      </c>
+      <c r="D142" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>265</v>
+      </c>
+      <c r="B143" t="s">
+        <v>137</v>
+      </c>
+      <c r="C143" t="s">
+        <v>102</v>
+      </c>
+      <c r="D143" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>206</v>
+      </c>
+      <c r="B144" t="s">
+        <v>137</v>
+      </c>
+      <c r="C144" t="s">
+        <v>38</v>
+      </c>
+      <c r="D144" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>268</v>
+      </c>
+      <c r="B145" t="s">
+        <v>137</v>
+      </c>
+      <c r="C145" t="s">
+        <v>102</v>
+      </c>
+      <c r="D145" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>270</v>
+      </c>
+      <c r="B146" t="s">
+        <v>137</v>
+      </c>
+      <c r="C146" t="s">
+        <v>102</v>
+      </c>
+      <c r="D146" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>207</v>
+      </c>
+      <c r="B147" t="s">
+        <v>137</v>
+      </c>
+      <c r="C147" t="s">
+        <v>38</v>
+      </c>
+      <c r="D147" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" t="s">
+        <v>137</v>
+      </c>
+      <c r="C148" t="s">
+        <v>38</v>
+      </c>
+      <c r="D148" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" t="s">
+        <v>137</v>
+      </c>
+      <c r="C149" t="s">
+        <v>38</v>
+      </c>
+      <c r="D149" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>274</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+      <c r="C150" t="s">
+        <v>102</v>
+      </c>
+      <c r="D150" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>275</v>
+      </c>
+      <c r="B151" t="s">
+        <v>137</v>
+      </c>
+      <c r="C151" t="s">
+        <v>102</v>
+      </c>
+      <c r="D151" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>277</v>
+      </c>
+      <c r="B152" t="s">
+        <v>137</v>
+      </c>
+      <c r="C152" t="s">
+        <v>102</v>
+      </c>
+      <c r="D152" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>210</v>
+      </c>
+      <c r="B153" t="s">
+        <v>137</v>
+      </c>
+      <c r="C153" t="s">
+        <v>38</v>
+      </c>
+      <c r="D153" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>211</v>
+      </c>
+      <c r="B154" t="s">
+        <v>137</v>
+      </c>
+      <c r="C154" t="s">
+        <v>38</v>
+      </c>
+      <c r="D154" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>280</v>
+      </c>
+      <c r="B155" t="s">
+        <v>137</v>
+      </c>
+      <c r="C155" t="s">
+        <v>102</v>
+      </c>
+      <c r="D155" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>212</v>
+      </c>
+      <c r="B156" t="s">
+        <v>137</v>
+      </c>
+      <c r="C156" t="s">
+        <v>38</v>
+      </c>
+      <c r="D156" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>282</v>
+      </c>
+      <c r="B157" t="s">
+        <v>137</v>
+      </c>
+      <c r="C157" t="s">
+        <v>102</v>
+      </c>
+      <c r="D157" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>285</v>
+      </c>
+      <c r="B158" t="s">
+        <v>137</v>
+      </c>
+      <c r="C158" t="s">
+        <v>102</v>
+      </c>
+      <c r="D158" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>213</v>
+      </c>
+      <c r="B159" t="s">
+        <v>137</v>
+      </c>
+      <c r="C159" t="s">
+        <v>38</v>
+      </c>
+      <c r="D159" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>289</v>
+      </c>
+      <c r="B160" t="s">
+        <v>137</v>
+      </c>
+      <c r="C160" t="s">
+        <v>102</v>
+      </c>
+      <c r="D160" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>214</v>
+      </c>
+      <c r="B161" t="s">
+        <v>137</v>
+      </c>
+      <c r="C161" t="s">
+        <v>38</v>
+      </c>
+      <c r="D161" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>